<commit_message>
Add Use case scenarios
</commit_message>
<xml_diff>
--- a/Task Manager - Report Outline.xlsx
+++ b/Task Manager - Report Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FinalProject\CampusMarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A975D77-1ECD-40A8-8984-F903D06B7E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E7793B-FB25-4961-B10C-7DC9CFA01DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t>Part1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -855,6 +855,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" s="7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Add UI-Admin Page - 1st Edition
</commit_message>
<xml_diff>
--- a/Task Manager - Report Outline.xlsx
+++ b/Task Manager - Report Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FinalProject\CampusMarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEC91A1-719A-4F73-AB96-198EE3B6B863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E44EC-7F42-4DA0-9D17-C7641EE15206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Admin-Manage Users-Use Case-01
</commit_message>
<xml_diff>
--- a/Task Manager - Report Outline.xlsx
+++ b/Task Manager - Report Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FinalProject\CampusMarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E44EC-7F42-4DA0-9D17-C7641EE15206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260A2163-F5F1-4893-B9BD-938B8658E148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t>Part1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t xml:space="preserve">  -Application Architecture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manage Users</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -770,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -841,352 +853,375 @@
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="D7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="C11" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="6" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C24" s="6" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C25" s="6" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D29" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C26" s="6" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C30" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C27" s="6" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="6" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="C33" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C30" s="6" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C31" s="6" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C32" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C37" s="6" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D39" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D40" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>